<commit_message>
Extraccion de texto mejorada, y guardado en el log
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\88891\Documents\UiPath\Archivaldo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beecker\Documents\UiPath\ArchivaldoBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3283A4D-0009-4B2B-83EB-6583BA0246FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -78,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,7 +436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">

</xml_diff>

<commit_message>
Validacion de documentos limpiada
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>No. Contrato</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>TipoContrato</t>
+  </si>
+  <si>
+    <t>la identificacion no le pernece al cliente</t>
+  </si>
+  <si>
+    <t>El estado de cuenta no se encuentra en la bd.</t>
+  </si>
+  <si>
+    <t>12/02/2020 09:31 a. m.;12/02/2020 09:31 a. m.;</t>
+  </si>
+  <si>
+    <t>00185537</t>
   </si>
 </sst>
 </file>
@@ -503,8 +515,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correccion de bug con el analisis de doctos
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se quito workflows inecesarios
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>No. Contrato</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>TipoContrato</t>
+  </si>
+  <si>
+    <t>la identificacion no le pernece al cliente</t>
+  </si>
+  <si>
+    <t>El estado de cuenta no se encuentra en la bd.</t>
+  </si>
+  <si>
+    <t>12/02/2020 09:31 a. m.;12/02/2020 09:31 a. m.;</t>
+  </si>
+  <si>
+    <t>00185537</t>
   </si>
 </sst>
 </file>
@@ -503,8 +515,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
validacion de doctos de nuevo funcionando
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>No. Contrato</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>TipoContrato</t>
-  </si>
-  <si>
-    <t>12/02/2020 09:31 a. m.;12/02/2020 09:31 a. m.;</t>
-  </si>
-  <si>
-    <t>00185537</t>
   </si>
 </sst>
 </file>
@@ -446,7 +440,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:M2"/>
+      <selection activeCell="H2" sqref="H2:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,12 +503,8 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregar cerrar caso al terminar el analisis
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Analisis de documentos terminado
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>No. Contrato</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>TipoContrato</t>
+  </si>
+  <si>
+    <t>ine ilegible</t>
+  </si>
+  <si>
+    <t>El estado de cuenta no se encuentra en la bd.</t>
+  </si>
+  <si>
+    <t>12/02/2020 09:31 a. m.;12/02/2020 09:31 a. m.;</t>
+  </si>
+  <si>
+    <t>00185537</t>
   </si>
 </sst>
 </file>
@@ -503,8 +515,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limpieza de check list
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>No. Contrato</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>TipoContrato</t>
+  </si>
+  <si>
+    <t>ine ilegible</t>
+  </si>
+  <si>
+    <t>validado</t>
+  </si>
+  <si>
+    <t>12/02/2020 09:31 a. m.;12/02/2020 09:31 a. m.;</t>
+  </si>
+  <si>
+    <t>00185537</t>
   </si>
 </sst>
 </file>
@@ -503,8 +515,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
validacion de solicitud terminada
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reconocimiento de casos hijos agregado
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>No. Contrato</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>TipoContrato</t>
+  </si>
+  <si>
+    <t>Figura</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AB12"/>
+      <selection activeCell="A2" sqref="A2:W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +455,7 @@
     <col min="12" max="12" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -495,8 +498,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I2" s="1"/>
       <c r="J2" s="2"/>
     </row>

</xml_diff>

<commit_message>
Validacion de curp corregida
</commit_message>
<xml_diff>
--- a/Data/LogClientes.xlsx
+++ b/Data/LogClientes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>No. Contrato</t>
   </si>
@@ -69,6 +69,33 @@
   </si>
   <si>
     <t>Figura</t>
+  </si>
+  <si>
+    <t>b.gabrielad@hotmail.com</t>
+  </si>
+  <si>
+    <t>validado</t>
+  </si>
+  <si>
+    <t>No coinciden el numero de cuenta que proporciono en su solicitud.</t>
+  </si>
+  <si>
+    <t>validado INE</t>
+  </si>
+  <si>
+    <t>5/03/2020 11:08 a. m.;</t>
+  </si>
+  <si>
+    <t>00185583</t>
+  </si>
+  <si>
+    <t>Casa de Bolsa</t>
+  </si>
+  <si>
+    <t>Discresional por asesoria</t>
+  </si>
+  <si>
+    <t>pf</t>
   </si>
 </sst>
 </file>
@@ -437,16 +464,16 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:R6"/>
+      <selection activeCell="A3" sqref="A3:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="35.140625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="39.28515625" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
@@ -503,8 +530,36 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>207375</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>